<commit_message>
reportes en excel y mantenimiento de contratas y listas
</commit_message>
<xml_diff>
--- a/DSiteBackend/src/main/resources/excel/CRM.xlsx
+++ b/DSiteBackend/src/main/resources/excel/CRM.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B3928-A302-4E8E-A946-0FDD50649AE1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E826E6E6-86C1-4CAE-8485-4F0EB447F1BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>Correlativo</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>Tipo de gasto</t>
   </si>
   <si>
-    <t>Fecha de Creaciòn</t>
-  </si>
-  <si>
     <t>Nombre Real</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Variación Oferta</t>
   </si>
   <si>
-    <t>Presupuesto Liquidacion</t>
-  </si>
-  <si>
     <t>Liquidación</t>
   </si>
   <si>
@@ -103,12 +94,6 @@
     <t>Factura Dsite</t>
   </si>
   <si>
-    <t>Variacón +</t>
-  </si>
-  <si>
-    <t>Variacón -</t>
-  </si>
-  <si>
     <t>Importe  de OCC</t>
   </si>
   <si>
@@ -116,13 +101,32 @@
   </si>
   <si>
     <t>NC</t>
+  </si>
+  <si>
+    <t>Variación +</t>
+  </si>
+  <si>
+    <t>Variación -</t>
+  </si>
+  <si>
+    <t>Presupuesto Liquidación</t>
+  </si>
+  <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Fecha de Creación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-10C6B]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +142,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,14 +186,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,122 +505,133 @@
     <col min="2" max="2" width="11.578125" customWidth="1"/>
     <col min="7" max="7" width="13.26171875" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="14" max="14" width="11.5234375" customWidth="1"/>
-    <col min="15" max="15" width="13.3125" customWidth="1"/>
-    <col min="18" max="18" width="12.3671875" customWidth="1"/>
-    <col min="19" max="19" width="12.05078125" customWidth="1"/>
-    <col min="20" max="20" width="10.68359375" customWidth="1"/>
+    <col min="10" max="10" width="8.83984375" style="3"/>
+    <col min="14" max="14" width="11.5234375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.26171875" customWidth="1"/>
+    <col min="16" max="16" width="13.15625" customWidth="1"/>
+    <col min="17" max="17" width="14.3125" customWidth="1"/>
+    <col min="18" max="18" width="16.68359375" customWidth="1"/>
+    <col min="19" max="19" width="15.41796875" customWidth="1"/>
+    <col min="20" max="20" width="14.9453125" customWidth="1"/>
     <col min="23" max="23" width="14.68359375" customWidth="1"/>
+    <col min="24" max="24" width="18.68359375" customWidth="1"/>
     <col min="26" max="26" width="10.3125" customWidth="1"/>
-    <col min="28" max="28" width="10.15625" customWidth="1"/>
+    <col min="28" max="28" width="14.3671875" customWidth="1"/>
+    <col min="29" max="29" width="16.89453125" customWidth="1"/>
+    <col min="30" max="30" width="14.83984375" customWidth="1"/>
     <col min="32" max="32" width="10.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:34" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>